<commit_message>
month and yearly data sets od CPI
</commit_message>
<xml_diff>
--- a/CPI.xlsx
+++ b/CPI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="980" windowWidth="28160" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,10 +341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C278" sqref="C278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -354,7 +353,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -365,116 +364,1436 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>11.010330701559001</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>13.4092895487289</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>14.720912024188401</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>16.713276338199002</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>20.588957549981</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>24.196656518752899</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>27.3982298355733</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>30.594532941416599</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>33.668024161160503</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>37.368989893888298</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>41.564397238272399</v>
+        <v>8.5544159743032395</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>45.373697680273601</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>49.660407175345902</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>55.776101677506396</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>63.472074398945502</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>70.752658185494994</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>77.373218876972501</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>87.759301763321105</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>94.642988552689303</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>100</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>104.88301248136899</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>109.60701436092801</v>
+        <v>11.010330701559001</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>11.010330701559001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>13.4092895487289</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>14.720912024188401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>16.713276338199002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>20.588957549981</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>24.196656518752899</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>27.3982298355733</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>30.594532941416599</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>33.668024161160503</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>37.368989893888298</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>41.564397238272399</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>45.373697680273601</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>49.660407175345902</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>55.776101677506396</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>63.472074398945502</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>70.752658185494994</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>77.373218876972501</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>87.759301763321105</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>94.642988552689303</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>104.88301248136899</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>109.60701436092801</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>115.333198124109</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289">
         <v>115.333198124109</v>
       </c>
     </row>

</xml_diff>